<commit_message>
Complete full api hey-payment
</commit_message>
<xml_diff>
--- a/documents/data-description.xlsx
+++ b/documents/data-description.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t xml:space="preserve">Key</t>
   </si>
@@ -83,6 +83,36 @@
   </si>
   <si>
     <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chuyển tiền thành công</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment → chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fullname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createdAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lucky→chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">session_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wish_message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">luckey_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type_message</t>
   </si>
 </sst>
 </file>
@@ -92,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -130,14 +160,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +178,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -198,7 +234,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,18 +259,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -282,7 +326,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -300,24 +344,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C1:F9"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="19" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.0333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="42.7259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.3592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="41.7444444444445"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.662962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="50.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="72.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="41.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,7 +421,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
@@ -388,7 +433,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
@@ -401,13 +446,14 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="6"/>
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="4"/>
@@ -424,10 +470,63 @@
       </c>
       <c r="F9" s="4"/>
     </row>
+    <row r="12" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>